<commit_message>
feat: first version of data files
</commit_message>
<xml_diff>
--- a/project/excel/food_system_indicators.xlsx
+++ b/project/excel/food_system_indicators.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="indicator" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="datapoint" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="quantity value" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="named thing" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="named thing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="indicator" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="indicator datapoint" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="indicator datapoint collection" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="quantity value" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,6 +417,47 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -427,33 +469,33 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>spatial scope</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>spatial scope</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>iri</t>
         </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Eu,EuMemberStates,Regional,Local"</formula1>
     </dataValidation>
   </dataValidations>
@@ -461,7 +503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -478,22 +520,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>measurement of</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has unit</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has numeric value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>datapoint of</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>has unit</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has numeric value</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -517,7 +559,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>indicator datapoints</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -566,45 +634,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>iri</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>